<commit_message>
nmf & lda revised and optimized
</commit_message>
<xml_diff>
--- a/Project_python/out/LDA/out_optimization.xlsx
+++ b/Project_python/out/LDA/out_optimization.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>test1.xlsx</t>
+          <t>test.xlsx</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -550,10 +550,10 @@
         <v>0.7</v>
       </c>
       <c r="N2" t="n">
-        <v>49.39024390243902</v>
+        <v>50</v>
       </c>
       <c r="O2" t="n">
-        <v>54.26829268292683</v>
+        <v>56.70731707317073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Texts for training reorganized
</commit_message>
<xml_diff>
--- a/Project_python/out/LDA/out_optimization.xlsx
+++ b/Project_python/out/LDA/out_optimization.xlsx
@@ -1,97 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upvedues-my.sharepoint.com/personal/alsanron_upv_edu_es/Documents/TFM/Repositories/NLP-SDGs_Classificator/Project_python/out/LDA/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_496DB2BFC07E2ACF6E03E0D741245E3FB48F8E71" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB98AF4F-9A79-4251-AF3B-A26D834ECD9A}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>num_topics</t>
-  </si>
-  <si>
-    <t>chunksize</t>
-  </si>
-  <si>
-    <t>passes</t>
-  </si>
-  <si>
-    <t>iterations</t>
-  </si>
-  <si>
-    <t>update_every</t>
-  </si>
-  <si>
-    <t>topics_csv</t>
-  </si>
-  <si>
-    <t>out_test_excel</t>
-  </si>
-  <si>
-    <t>score_threshold</t>
-  </si>
-  <si>
-    <t>only_bad</t>
-  </si>
-  <si>
-    <t>only_positive</t>
-  </si>
-  <si>
-    <t>min_words_count</t>
-  </si>
-  <si>
-    <t>max_words_frequency</t>
-  </si>
-  <si>
-    <t>perc_global</t>
-  </si>
-  <si>
-    <t>perc_any</t>
-  </si>
-  <si>
-    <t>lda_topics.csv</t>
-  </si>
-  <si>
-    <t>test.xlsx</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -106,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -430,89 +420,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>num_topics</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>chunksize</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>passes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>iterations</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>update_every</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>topics_csv</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>out_test_excel</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>score_threshold</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>only_bad</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>only_positive</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>min_words_count</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>max_words_frequency</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>perc_global</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>perc_any</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
+        <v>17</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>400</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>2000</v>
-      </c>
-      <c r="D2">
-        <v>400</v>
-      </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>lda_topics.csv</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>test.xlsx</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
         <v>0.2</v>
       </c>
       <c r="J2" t="b">
@@ -521,17 +543,17 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="L2" t="n">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="n">
         <v>0.7</v>
       </c>
-      <c r="N2">
-        <v>71.341463414634148</v>
-      </c>
-      <c r="O2">
-        <v>76.829268292682926</v>
+      <c r="N2" t="n">
+        <v>56.70731707317073</v>
+      </c>
+      <c r="O2" t="n">
+        <v>64.02439024390245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>